<commit_message>
yet more reorganizing and refactoring
</commit_message>
<xml_diff>
--- a/component-sourcing/OSCHISP_electrical_BOM_opta_v1.0.xlsx
+++ b/component-sourcing/OSCHISP_electrical_BOM_opta_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FAST Research Group\Heat Processes Projects\Mini Press 1000\open-source-cold-and-hot-scientific-sheet-press\component-sourcing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C90D8E9-4E74-4C7F-88EC-20A131649166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15ABE5A-B25A-4684-A20C-49F80380B93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>https://www.digikey.ca/en/products/detail/weidm%C3%BCller/1024100000/497593</t>
   </si>
@@ -70,6 +70,39 @@
   </si>
   <si>
     <t>Relay 4</t>
+  </si>
+  <si>
+    <t>Thermocouple DIN Rail Terminal Blocks, Narrow 10.7 mm Width</t>
+  </si>
+  <si>
+    <t>https://www.omega.com/en-us/temperature-measurement/temperature-connectors-panels-and-block-assemblies/terminal-blocks-and-lugs/drtb-2/p/DRTB-T-2</t>
+  </si>
+  <si>
+    <t>Thermocouple DIN Terminal Block Connector 2 Position Feed Through Beige 12-26 AWG</t>
+  </si>
+  <si>
+    <t>DIN Rail Thermocouple Input Signal Conditioners | Low Profile</t>
+  </si>
+  <si>
+    <t>https://www.omega.com/en-us/data-acquisition/signal-conditioners/din-rail-signal-conditioners/p/DRSL-TC-Srs-Sig-Cond</t>
+  </si>
+  <si>
+    <t>STATUS SEM1605/TC, TEMP TRANSMITTER, THERMOCOUPLE, DIN RAIL</t>
+  </si>
+  <si>
+    <t>https://www.newark.com/status/sem1605-tc/temp-transmitter-thermocouple/dp/13AC9411?MER=TARG-MER-PDP-RECO-STM71168</t>
+  </si>
+  <si>
+    <t>SENECA WK109TC0 SIGNAL CONDITIONER, FOR THEROCOUPLES</t>
+  </si>
+  <si>
+    <t>https://www.newark.com/seneca/wk109tc0/signal-conditioner-for-therocouples/dp/24M9179</t>
+  </si>
+  <si>
+    <t>Portenta Machine Control</t>
+  </si>
+  <si>
+    <t>https://store-usa.arduino.cc/products/arduino-portenta-machine-control?selectedStore=us</t>
   </si>
 </sst>
 </file>
@@ -120,9 +153,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -404,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C6D00D-4364-434A-BC00-F15762E94AA1}">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A2:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +512,54 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -486,6 +570,12 @@
     <hyperlink ref="B7" r:id="rId5" xr:uid="{9D8A4A81-331F-4C51-A48A-65F5C5407CD8}"/>
     <hyperlink ref="B8" r:id="rId6" xr:uid="{989F6291-BF10-4D02-BA04-C281C0F1CD61}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{5815DEE5-FD92-4C7A-B1D4-1F0FE1AD906C}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{77BFD672-867D-4606-86B2-51EDFDE26E6E}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{24BC43E8-DAB7-4369-8133-8C6C368F5664}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{A25EA387-3D01-452F-AA02-1942F1E986B0}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{E1929B6C-E56E-4548-869F-D83D23BC335F}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{9C57D1F1-B306-40A2-A370-CD5EF17BB1C9}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{838A42B8-C2CF-45BF-BA4A-96D53473165B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>